<commit_message>
Cleaned up project and updated files
</commit_message>
<xml_diff>
--- a/SDDI-Metadata.xlsx
+++ b/SDDI-Metadata.xlsx
@@ -1703,7 +1703,7 @@
     <row r="8" ht="15.75" customHeight="1" s="25">
       <c r="E8" s="24" t="inlineStr">
         <is>
-          <t>Digitaler Zwilling</t>
+          <t>Datensatz und Dokumente</t>
         </is>
       </c>
       <c r="G8" s="24" t="inlineStr">
@@ -1725,7 +1725,7 @@
     <row r="9" ht="15.75" customHeight="1" s="25">
       <c r="E9" s="24" t="inlineStr">
         <is>
-          <t>Energie</t>
+          <t>Digitaler Zwilling</t>
         </is>
       </c>
       <c r="G9" s="24" t="inlineStr">
@@ -1742,7 +1742,7 @@
     <row r="10" ht="15.75" customHeight="1" s="25">
       <c r="E10" s="24" t="inlineStr">
         <is>
-          <t>Geoobjekt</t>
+          <t>Energie</t>
         </is>
       </c>
       <c r="G10" s="24" t="inlineStr">
@@ -1759,7 +1759,7 @@
     <row r="11" ht="15.75" customHeight="1" s="25">
       <c r="E11" s="24" t="inlineStr">
         <is>
-          <t>Gerät / Ding</t>
+          <t>Geoobjekt</t>
         </is>
       </c>
       <c r="G11" s="24" t="inlineStr">
@@ -1776,7 +1776,7 @@
     <row r="12" ht="15.75" customHeight="1" s="25">
       <c r="E12" s="24" t="inlineStr">
         <is>
-          <t>Gesundheit</t>
+          <t>Gerät / Ding</t>
         </is>
       </c>
       <c r="G12" s="24" t="inlineStr">
@@ -1793,7 +1793,7 @@
     <row r="13" ht="15.75" customHeight="1" s="25">
       <c r="E13" s="24" t="inlineStr">
         <is>
-          <t>Gewerbe / Handwerk</t>
+          <t>Gesundheit</t>
         </is>
       </c>
       <c r="G13" s="24" t="inlineStr">
@@ -1810,7 +1810,7 @@
     <row r="14" ht="15.75" customHeight="1" s="25">
       <c r="E14" s="24" t="inlineStr">
         <is>
-          <t>Handel</t>
+          <t>Gewerbe / Handwerk</t>
         </is>
       </c>
       <c r="G14" s="24" t="inlineStr">
@@ -1827,7 +1827,7 @@
     <row r="15" ht="15.75" customHeight="1" s="25">
       <c r="E15" s="24" t="inlineStr">
         <is>
-          <t>Hauptkategorien</t>
+          <t>Handel</t>
         </is>
       </c>
       <c r="G15" s="24" t="inlineStr">
@@ -1844,7 +1844,7 @@
     <row r="16" ht="15.75" customHeight="1" s="25">
       <c r="E16" s="24" t="inlineStr">
         <is>
-          <t>Informations-Technologie</t>
+          <t>Hauptkategorien</t>
         </is>
       </c>
       <c r="G16" s="24" t="inlineStr">
@@ -1861,7 +1861,7 @@
     <row r="17" ht="15.75" customHeight="1" s="25">
       <c r="E17" s="24" t="inlineStr">
         <is>
-          <t>Kultur</t>
+          <t>Informations-Technologie</t>
         </is>
       </c>
       <c r="G17" s="24" t="inlineStr">
@@ -1878,7 +1878,7 @@
     <row r="18" ht="15.75" customHeight="1" s="25">
       <c r="E18" s="24" t="inlineStr">
         <is>
-          <t>Landwirtschaft</t>
+          <t>Kultur</t>
         </is>
       </c>
       <c r="G18" s="24" t="inlineStr">
@@ -1895,7 +1895,7 @@
     <row r="19" ht="15.75" customHeight="1" s="25">
       <c r="E19" s="24" t="inlineStr">
         <is>
-          <t>Methode</t>
+          <t>Landwirtschaft</t>
         </is>
       </c>
       <c r="G19" s="24" t="inlineStr">
@@ -1912,7 +1912,7 @@
     <row r="20" ht="15.75" customHeight="1" s="25">
       <c r="E20" s="24" t="inlineStr">
         <is>
-          <t>Mobilität</t>
+          <t>Methode</t>
         </is>
       </c>
       <c r="G20" s="24" t="inlineStr">
@@ -1929,7 +1929,7 @@
     <row r="21" ht="15.75" customHeight="1" s="25">
       <c r="E21" s="24" t="inlineStr">
         <is>
-          <t>Online-Anwendung</t>
+          <t>Mobilität</t>
         </is>
       </c>
       <c r="G21" s="24" t="inlineStr">
@@ -1946,7 +1946,7 @@
     <row r="22" ht="15.75" customHeight="1" s="25">
       <c r="E22" s="24" t="inlineStr">
         <is>
-          <t>Online-Dienst</t>
+          <t>Online-Anwendung</t>
         </is>
       </c>
       <c r="G22" s="24" t="inlineStr">
@@ -1963,7 +1963,7 @@
     <row r="23" ht="15.75" customHeight="1" s="25">
       <c r="E23" s="24" t="inlineStr">
         <is>
-          <t>Projekt</t>
+          <t>Online-Dienst</t>
         </is>
       </c>
       <c r="G23" s="24" t="inlineStr">
@@ -1975,42 +1975,42 @@
     <row r="24" ht="15.75" customHeight="1" s="25">
       <c r="E24" s="24" t="inlineStr">
         <is>
-          <t>Software</t>
+          <t>Projekt</t>
         </is>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1" s="25">
       <c r="E25" s="24" t="inlineStr">
         <is>
-          <t>Stadtplanung</t>
+          <t>Software</t>
         </is>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1" s="25">
       <c r="E26" s="24" t="inlineStr">
         <is>
-          <t>Themen</t>
+          <t>Stadtplanung</t>
         </is>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1" s="25">
       <c r="E27" s="24" t="inlineStr">
         <is>
-          <t>Tourismus &amp; Freizeit</t>
+          <t>Themen</t>
         </is>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1" s="25">
       <c r="E28" s="24" t="inlineStr">
         <is>
-          <t>Umwelt</t>
+          <t>Tourismus &amp; Freizeit</t>
         </is>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1" s="25">
       <c r="E29" s="24" t="inlineStr">
         <is>
-          <t>Verwaltung</t>
+          <t>Umwelt</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
PoC version, automate registration from excel sheet detection
</commit_message>
<xml_diff>
--- a/SDDI-Metadata.xlsx
+++ b/SDDI-Metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="24750" windowHeight="12200" activeTab="7"/>
+    <workbookView windowWidth="24750" windowHeight="12200" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Data Mapping" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="275">
   <si>
     <t>Hauptkategorien</t>
   </si>
@@ -735,6 +735,9 @@
     <t>Test Maintainer</t>
   </si>
   <si>
+    <t>error test</t>
+  </si>
+  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -874,6 +877,9 @@
   </si>
   <si>
     <t>Example Software 1</t>
+  </si>
+  <si>
+    <t>This is an example software</t>
   </si>
   <si>
     <t>4gb</t>
@@ -908,18 +914,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1059,7 +1065,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1117,12 +1123,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1389,28 +1389,28 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1461,87 +1461,86 @@
     <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1933,7 +1932,7 @@
   <sheetPr/>
   <dimension ref="A1:AF33"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB1" sqref="AB1:AB4"/>
     </sheetView>
   </sheetViews>
@@ -1991,7 +1990,7 @@
       <c r="M1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="7"/>
+      <c r="N1" s="6"/>
       <c r="O1" s="5" t="s">
         <v>11</v>
       </c>
@@ -2001,7 +2000,7 @@
       <c r="Q1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="7"/>
+      <c r="R1" s="6"/>
       <c r="S1" s="5" t="s">
         <v>14</v>
       </c>
@@ -2011,7 +2010,7 @@
       <c r="U1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="7"/>
+      <c r="V1" s="6"/>
       <c r="W1" s="5" t="s">
         <v>17</v>
       </c>
@@ -2021,11 +2020,11 @@
       <c r="Z1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" s="7"/>
+      <c r="AA1" s="6"/>
       <c r="AB1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="AC1" s="7"/>
+      <c r="AC1" s="6"/>
       <c r="AD1" s="5" t="s">
         <v>21</v>
       </c>
@@ -2040,7 +2039,7 @@
       <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" t="s">
         <v>25</v>
       </c>
       <c r="E2" t="s">
@@ -2070,13 +2069,12 @@
       <c r="O2" t="s">
         <v>33</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" t="s">
         <v>35</v>
       </c>
-      <c r="R2" s="6"/>
       <c r="S2" t="s">
         <v>36</v>
       </c>
@@ -2112,13 +2110,13 @@
       <c r="C3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" t="s">
         <v>46</v>
       </c>
       <c r="E3" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" t="s">
         <v>48</v>
       </c>
       <c r="H3" t="s">
@@ -2136,16 +2134,15 @@
       <c r="L3" t="s">
         <v>53</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" t="s">
         <v>54</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" t="s">
         <v>55</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" t="s">
         <v>56</v>
       </c>
-      <c r="R3" s="6"/>
       <c r="S3" t="s">
         <v>57</v>
       </c>
@@ -2196,30 +2193,28 @@
       <c r="K4" t="s">
         <v>71</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" t="s">
         <v>72</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" t="s">
         <v>73</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="Q4" t="s">
         <v>74</v>
       </c>
-      <c r="R4" s="6"/>
       <c r="S4" t="s">
         <v>75</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="T4" t="s">
         <v>76</v>
       </c>
-      <c r="U4" s="6" t="s">
+      <c r="U4" t="s">
         <v>77</v>
       </c>
-      <c r="V4" s="6"/>
       <c r="W4" t="s">
         <v>78</v>
       </c>
-      <c r="Y4" s="6" t="s">
+      <c r="Y4" t="s">
         <v>79</v>
       </c>
       <c r="Z4" t="s">
@@ -2257,16 +2252,15 @@
       <c r="K5" t="s">
         <v>88</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="O5" t="s">
         <v>89</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="P5" t="s">
         <v>90</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="Q5" t="s">
         <v>91</v>
       </c>
-      <c r="R5" s="6"/>
       <c r="T5" t="s">
         <v>92</v>
       </c>
@@ -2504,10 +2498,9 @@
       <c r="H14" t="s">
         <v>160</v>
       </c>
-      <c r="T14" s="6" t="s">
+      <c r="T14" t="s">
         <v>78</v>
       </c>
-      <c r="V14" s="6"/>
       <c r="AD14" t="s">
         <v>161</v>
       </c>
@@ -2640,15 +2633,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="U1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="AA2" sqref="AA2:AC2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
   <cols>
     <col min="1" max="1" width="21.0833333333333" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.25" style="2" customWidth="1"/>
@@ -2801,7 +2794,7 @@
       <c r="I2" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -2813,7 +2806,7 @@
       <c r="M2" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="O2" s="2" t="s">
@@ -2846,10 +2839,9 @@
       <c r="X2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Z2" s="4"/>
       <c r="AA2" s="2" t="s">
         <v>218</v>
       </c>
@@ -2894,7 +2886,7 @@
       <c r="I3" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="2" t="s">
         <v>48</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -2943,6 +2935,86 @@
         <v>32</v>
       </c>
       <c r="AE3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" ht="60" customHeight="1" spans="1:31">
+      <c r="A4" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE4" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2994,6 +3066,9 @@
       <formula1>Privacy_Policy</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="H4" r:id="rId1" display="max-mustermann@gmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
@@ -3117,16 +3192,16 @@
         <v>8</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>14</v>
@@ -3135,16 +3210,16 @@
         <v>15</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>10</v>
@@ -3167,7 +3242,7 @@
     </row>
     <row r="2" ht="44" customHeight="1" spans="1:38">
       <c r="A2" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -3218,7 +3293,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -3236,7 +3311,7 @@
         <v>37</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="AD2" s="2" t="s">
         <v>38</v>
@@ -3262,7 +3337,7 @@
     </row>
     <row r="3" ht="46.5" customHeight="1" spans="1:38">
       <c r="A3" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -3313,7 +3388,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -3341,8 +3416,8 @@
       </c>
     </row>
     <row r="4" spans="1:38">
-      <c r="A4" s="4" t="s">
-        <v>235</v>
+      <c r="A4" s="2" t="s">
+        <v>236</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>209</v>
@@ -3366,7 +3441,7 @@
         <v>212</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>27</v>
@@ -3384,7 +3459,7 @@
         <v>25</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>29</v>
@@ -3561,7 +3636,7 @@
         <v>8</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>203</v>
@@ -3581,7 +3656,7 @@
     </row>
     <row r="2" spans="1:28">
       <c r="A2" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -3632,7 +3707,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -3661,7 +3736,7 @@
     </row>
     <row r="3" spans="1:28">
       <c r="A3" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -3712,7 +3787,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -3863,16 +3938,16 @@
         <v>8</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>10</v>
@@ -3895,7 +3970,7 @@
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -3946,7 +4021,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -3973,7 +4048,7 @@
         <v>97</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>220</v>
@@ -3984,7 +4059,7 @@
     </row>
     <row r="3" spans="1:32">
       <c r="A3" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -4035,7 +4110,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -4057,8 +4132,8 @@
       </c>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="4" t="s">
-        <v>247</v>
+      <c r="A4" s="2" t="s">
+        <v>248</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>209</v>
@@ -4109,7 +4184,7 @@
         <v>216</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>53</v>
@@ -4267,13 +4342,13 @@
         <v>17</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>10</v>
@@ -4296,7 +4371,7 @@
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -4347,7 +4422,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -4365,7 +4440,7 @@
         <v>36</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>32</v>
@@ -4377,7 +4452,7 @@
         <v>97</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>220</v>
@@ -4388,7 +4463,7 @@
     </row>
     <row r="3" spans="1:32">
       <c r="A3" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -4439,7 +4514,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -4512,8 +4587,8 @@
   <sheetPr/>
   <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
@@ -4596,7 +4671,7 @@
         <v>18</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>19</v>
@@ -4625,7 +4700,7 @@
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -4676,7 +4751,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -4694,9 +4769,9 @@
         <v>36</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="Y2" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>42</v>
       </c>
       <c r="Z2" s="2" t="s">
@@ -4709,7 +4784,7 @@
         <v>97</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>220</v>
@@ -4720,7 +4795,7 @@
     </row>
     <row r="3" spans="1:32">
       <c r="A3" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -4771,7 +4846,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -4802,8 +4877,8 @@
       </c>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="4" t="s">
-        <v>258</v>
+      <c r="A4" s="2" t="s">
+        <v>259</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>209</v>
@@ -4854,7 +4929,7 @@
         <v>216</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>53</v>
@@ -4939,7 +5014,7 @@
   <sheetPr/>
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
@@ -5023,7 +5098,7 @@
         <v>8</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>10</v>
@@ -5046,7 +5121,7 @@
     </row>
     <row r="2" spans="1:29">
       <c r="A2" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -5097,7 +5172,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -5121,7 +5196,7 @@
         <v>97</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AB2" s="2" t="s">
         <v>220</v>
@@ -5132,7 +5207,7 @@
     </row>
     <row r="3" spans="1:29">
       <c r="A3" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -5183,7 +5258,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -5206,7 +5281,7 @@
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>209</v>
@@ -5255,7 +5330,7 @@
         <v>216</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>53</v>
@@ -5278,41 +5353,41 @@
     </row>
   </sheetData>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4 D1:D3 D5:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D$1:D$1048576">
       <formula1>'Data Mapping'!$H:$H</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4 J1:J3 J5:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J$1:J$1048576">
       <formula1>'Data Mapping'!$F:$F</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4 K1:K3 K5:K1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K$1:K$1048576">
       <formula1>'Data Mapping'!$E:$E</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4 L1:L3 L5:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L$1:L$1048576">
       <formula1>'Data Mapping'!$A$9</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M4 M1:M3 M5:M1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M$1:M$1048576">
       <formula1>'Data Mapping'!$C:$C</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N4 N1:N3 N5:N1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N$1:N$1048576">
       <formula1>'Data Mapping'!$D:$D</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S4 S1:S3 S5:S1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S$1:S$1048576">
       <formula1>'Data Mapping'!$L:$L</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T4 T1:T3 T5:T1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T$1:T$1048576">
       <formula1>'Data Mapping'!$J:$J</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U4 U1:U3 U5:U1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U$1:U$1048576">
       <formula1>'Data Mapping'!$K:$K</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V4 V1:V3 V5:V1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V$1:V$1048576">
       <formula1>'Data Mapping'!$AD:$AD</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W4:X4 W1:X3 W5:X1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC$1:AC$1048576">
+      <formula1>'Data Mapping'!$I:$I</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W$1:X$1048576">
       <formula1>Privacy_Policy</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC4 AC1:AC3 AC5:AC1048576">
-      <formula1>'Data Mapping'!$I:$I</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5325,22 +5400,28 @@
   <sheetPr/>
   <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
       <selection activeCell="AF5" sqref="AF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="3" width="9" style="2"/>
+    <col min="1" max="1" width="30.3333333333333" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.4166666666667" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.25" style="2" customWidth="1"/>
     <col min="4" max="4" width="29.0833333333333" style="2" customWidth="1"/>
     <col min="5" max="9" width="9" style="2"/>
     <col min="10" max="10" width="15.1666666666667" style="2" customWidth="1"/>
     <col min="11" max="11" width="25.3333333333333" style="2" customWidth="1"/>
-    <col min="12" max="22" width="9" style="2"/>
+    <col min="12" max="18" width="9" style="2"/>
+    <col min="19" max="19" width="18.5" style="2" customWidth="1"/>
+    <col min="20" max="22" width="9" style="2"/>
     <col min="23" max="23" width="16.5833333333333" style="2" customWidth="1"/>
     <col min="24" max="28" width="9" style="2"/>
-    <col min="29" max="30" width="26.3333333333333" style="2" customWidth="1"/>
-    <col min="31" max="16384" width="9" style="2"/>
+    <col min="29" max="29" width="26.3333333333333" style="2" customWidth="1"/>
+    <col min="30" max="30" width="7.25" style="2" customWidth="1"/>
+    <col min="31" max="31" width="19.8333333333333" style="2" customWidth="1"/>
+    <col min="32" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="26" customHeight="1" spans="1:35">
@@ -5411,22 +5492,22 @@
         <v>22</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>10</v>
@@ -5449,7 +5530,7 @@
     </row>
     <row r="2" spans="1:35">
       <c r="A2" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -5482,7 +5563,7 @@
         <v>111</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>137</v>
@@ -5500,7 +5581,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -5515,10 +5596,10 @@
         <v>39</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>32</v>
@@ -5530,7 +5611,7 @@
         <v>97</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AH2" s="2" t="s">
         <v>220</v>
@@ -5541,16 +5622,16 @@
     </row>
     <row r="3" spans="1:35">
       <c r="A3" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>209</v>
+        <v>272</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>210</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>49</v>
+        <v>132</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>222</v>
@@ -5571,10 +5652,10 @@
         <v>48</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>111</v>
+        <v>47</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>137</v>
@@ -5592,7 +5673,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -5607,13 +5688,22 @@
         <v>39</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="AC3" s="2" t="s">
         <v>32</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>219</v>
       </c>
       <c r="AI3" s="2" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
modify the creating logics
</commit_message>
<xml_diff>
--- a/SDDI-Metadata.xlsx
+++ b/SDDI-Metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="24750" windowHeight="12200" activeTab="8"/>
+    <workbookView windowWidth="24750" windowHeight="12200" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Data Mapping" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="276">
   <si>
     <t>Hauptkategorien</t>
   </si>
@@ -714,9 +714,6 @@
     <t>2025-07-20</t>
   </si>
   <si>
-    <t>München</t>
-  </si>
-  <si>
     <t>https://dz.forchheim.de/#/</t>
   </si>
   <si>
@@ -738,6 +735,9 @@
     <t>error test</t>
   </si>
   <si>
+    <t>Example Dataset new test</t>
+  </si>
+  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -826,6 +826,9 @@
   </si>
   <si>
     <t>Example Online Application 1</t>
+  </si>
+  <si>
+    <t>Example Online Application 727</t>
   </si>
   <si>
     <t>API Endpoint</t>
@@ -2625,7 +2628,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="H4:I19 H1 A5:A6 H2:I2 I3 K18:K19" numberStoredAsText="1"/>
+    <ignoredError sqref="K18:K19 I3 H2:I2 A5:A6 H1 H4:I19" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2633,17 +2636,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AE4"/>
+  <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="AA2" sqref="AA2:AC2"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4"/>
   <cols>
-    <col min="1" max="1" width="21.0833333333333" style="2" customWidth="1"/>
+    <col min="1" max="1" width="51.75" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.25" style="2" customWidth="1"/>
     <col min="3" max="3" width="17.25" style="2" customWidth="1"/>
     <col min="4" max="4" width="31.25" style="2" customWidth="1"/>
@@ -2818,9 +2821,6 @@
       <c r="Q2" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
       </c>
@@ -2843,16 +2843,16 @@
         <v>32</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AB2" s="2" t="s">
         <v>97</v>
       </c>
       <c r="AC2" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="AD2" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>29</v>
@@ -2860,7 +2860,7 @@
     </row>
     <row r="3" ht="60" customHeight="1" spans="1:31">
       <c r="A3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -2872,13 +2872,13 @@
         <v>132</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>212</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>212</v>
@@ -2910,9 +2910,6 @@
       <c r="Q3" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
       </c>
@@ -2940,7 +2937,7 @@
     </row>
     <row r="4" ht="60" customHeight="1" spans="1:31">
       <c r="A4" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>209</v>
@@ -2952,13 +2949,13 @@
         <v>132</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>212</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>212</v>
@@ -2990,9 +2987,6 @@
       <c r="Q4" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="R4" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="S4" s="2" t="s">
         <v>53</v>
       </c>
@@ -3015,6 +3009,83 @@
         <v>32</v>
       </c>
       <c r="AE4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" ht="60" customHeight="1" spans="1:31">
+      <c r="A5" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE5" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3072,7 +3143,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="AC1:AD1 AA1 E1:I3 O1:R3 AA2:AD3 A1:C3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:C3 AA2:AD3 O2:Q3 O1:R1 E1:I3 AA1 AC1:AD1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3320,16 +3391,16 @@
         <v>32</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AI2" s="2" t="s">
         <v>97</v>
       </c>
       <c r="AJ2" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="AK2" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="AL2" s="2" t="s">
         <v>29</v>
@@ -3349,13 +3420,13 @@
         <v>132</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>212</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>212</v>
@@ -3429,13 +3500,13 @@
         <v>68</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>212</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>212</v>
@@ -3719,16 +3790,16 @@
         <v>71</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>97</v>
       </c>
       <c r="Z2" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA2" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="AB2" s="2" t="s">
         <v>184</v>
@@ -3748,13 +3819,13 @@
         <v>132</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>212</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>212</v>
@@ -4042,7 +4113,7 @@
         <v>32</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>97</v>
@@ -4051,7 +4122,7 @@
         <v>246</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AF2" s="2" t="s">
         <v>6</v>
@@ -4071,13 +4142,13 @@
         <v>132</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>212</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>212</v>
@@ -4145,13 +4216,13 @@
         <v>150</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>212</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>212</v>
@@ -4255,13 +4326,13 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
   <cols>
     <col min="1" max="1" width="16.1666666666667" style="2" customWidth="1"/>
     <col min="2" max="3" width="9" style="2"/>
@@ -4446,7 +4517,7 @@
         <v>32</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>97</v>
@@ -4455,7 +4526,7 @@
         <v>246</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AF2" s="2" t="s">
         <v>184</v>
@@ -4475,13 +4546,13 @@
         <v>132</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>212</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>212</v>
@@ -4538,43 +4609,120 @@
         <v>184</v>
       </c>
     </row>
+    <row r="4" spans="1:32">
+      <c r="A4" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D$1:D$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4 D1:D3 D5:D1048576">
       <formula1>'Data Mapping'!$H:$H</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J$1:J$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4 J1:J3 J5:J1048576">
       <formula1>'Data Mapping'!$F:$F</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K$1:K$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4 K1:K3 K5:K1048576">
       <formula1>'Data Mapping'!$E:$E</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L$1:L$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4 L1:L3 L5:L1048576">
       <formula1>'Data Mapping'!$A$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M$1:M$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M4 M1:M3 M5:M1048576">
       <formula1>'Data Mapping'!$C:$C</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N$1:N$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N4 N1:N3 N5:N1048576">
       <formula1>'Data Mapping'!$D:$D</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S$1:S$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S4 S1:S3 S5:S1048576">
       <formula1>'Data Mapping'!$L:$L</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T$1:T$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T4 T1:T3 T5:T1048576">
       <formula1>'Data Mapping'!$J:$J</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U$1:U$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U4 U1:U3 U5:U1048576">
       <formula1>'Data Mapping'!$K:$K</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V$1:V$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V4 V1:V3 V5:V1048576">
       <formula1>'Data Mapping'!$W:$W</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF$1:AF$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z4:AA4 Z1:AA3 Z5:AA1048576">
+      <formula1>Privacy_Policy</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF4 AF1:AF3 AF5:AF1048576">
       <formula1>'Data Mapping'!$I:$I</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z$1:AA$1048576">
-      <formula1>Privacy_Policy</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4671,7 +4819,7 @@
         <v>18</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>19</v>
@@ -4700,7 +4848,7 @@
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -4769,7 +4917,7 @@
         <v>36</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>42</v>
@@ -4778,7 +4926,7 @@
         <v>32</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>97</v>
@@ -4787,7 +4935,7 @@
         <v>246</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AF2" s="2" t="s">
         <v>29</v>
@@ -4795,7 +4943,7 @@
     </row>
     <row r="3" spans="1:32">
       <c r="A3" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -4807,13 +4955,13 @@
         <v>132</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>212</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>212</v>
@@ -4878,7 +5026,7 @@
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>209</v>
@@ -4890,13 +5038,13 @@
         <v>132</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>212</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>212</v>
@@ -5098,7 +5246,7 @@
         <v>8</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>10</v>
@@ -5121,7 +5269,7 @@
     </row>
     <row r="2" spans="1:29">
       <c r="A2" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -5190,7 +5338,7 @@
         <v>32</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>97</v>
@@ -5199,7 +5347,7 @@
         <v>246</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>29</v>
@@ -5207,7 +5355,7 @@
     </row>
     <row r="3" spans="1:29">
       <c r="A3" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -5219,13 +5367,13 @@
         <v>49</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>212</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>212</v>
@@ -5281,7 +5429,7 @@
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>209</v>
@@ -5293,13 +5441,13 @@
         <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>212</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>212</v>
@@ -5400,7 +5548,7 @@
   <sheetPr/>
   <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+    <sheetView topLeftCell="S1" workbookViewId="0">
       <selection activeCell="AF5" sqref="AF5"/>
     </sheetView>
   </sheetViews>
@@ -5492,19 +5640,19 @@
         <v>22</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>250</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>251</v>
@@ -5530,7 +5678,7 @@
     </row>
     <row r="2" spans="1:35">
       <c r="A2" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -5596,16 +5744,16 @@
         <v>39</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AF2" s="2" t="s">
         <v>97</v>
@@ -5614,7 +5762,7 @@
         <v>246</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AI2" s="2" t="s">
         <v>29</v>
@@ -5622,10 +5770,10 @@
     </row>
     <row r="3" spans="1:35">
       <c r="A3" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>210</v>
@@ -5634,13 +5782,13 @@
         <v>132</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>212</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>212</v>
@@ -5688,22 +5836,22 @@
         <v>39</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AC3" s="2" t="s">
         <v>32</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AF3" s="2" t="s">
         <v>97</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AI3" s="2" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
remove unused functions in creat.py
</commit_message>
<xml_diff>
--- a/SDDI-Metadata.xlsx
+++ b/SDDI-Metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="24750" windowHeight="12200" activeTab="5"/>
+    <workbookView windowWidth="24750" windowHeight="12200" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data Mapping" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="279">
   <si>
     <t>Hauptkategorien</t>
   </si>
@@ -738,6 +738,12 @@
     <t>Example Dataset new test</t>
   </si>
   <si>
+    <t xml:space="preserve">Example Dataset84 </t>
+  </si>
+  <si>
+    <t>This is today dataset</t>
+  </si>
+  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -778,6 +784,9 @@
   </si>
   <si>
     <t>1.1</t>
+  </si>
+  <si>
+    <t>Example Device 84</t>
   </si>
   <si>
     <t>Simulation Model</t>
@@ -2636,15 +2645,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AE5"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="$A6:$XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="51.75" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.25" style="2" customWidth="1"/>
@@ -3089,6 +3098,83 @@
         <v>29</v>
       </c>
     </row>
+    <row r="6" ht="60" customHeight="1" spans="1:31">
+      <c r="A6" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="15">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1 L3:L1048576">
@@ -3151,15 +3237,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AL4"/>
+  <dimension ref="A1:AL5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="$A4:$XFD4"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="$A5:$XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4"/>
   <cols>
     <col min="1" max="1" width="17.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="22" style="2" customWidth="1"/>
@@ -3263,16 +3349,16 @@
         <v>8</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>14</v>
@@ -3281,16 +3367,16 @@
         <v>15</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>10</v>
@@ -3313,7 +3399,7 @@
     </row>
     <row r="2" ht="44" customHeight="1" spans="1:38">
       <c r="A2" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -3364,7 +3450,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -3382,7 +3468,7 @@
         <v>37</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="AD2" s="2" t="s">
         <v>38</v>
@@ -3408,7 +3494,7 @@
     </row>
     <row r="3" ht="46.5" customHeight="1" spans="1:38">
       <c r="A3" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -3459,7 +3545,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -3488,7 +3574,7 @@
     </row>
     <row r="4" spans="1:38">
       <c r="A4" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>209</v>
@@ -3512,7 +3598,7 @@
         <v>212</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>27</v>
@@ -3530,7 +3616,7 @@
         <v>25</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>29</v>
@@ -3557,49 +3643,120 @@
         <v>29</v>
       </c>
     </row>
+    <row r="5" spans="1:38">
+      <c r="A5" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="14">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D$1:D$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D1:D4 D6:D1048576">
       <formula1>'Data Mapping'!$H:$H</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J$1:J$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5 J1:J4 J6:J1048576">
       <formula1>'Data Mapping'!$F:$F</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K$1:K$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5 K1:K4 K6:K1048576">
       <formula1>'Data Mapping'!$E:$E</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L$1:L$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5 L1:L4 L6:L1048576">
       <formula1>'Data Mapping'!$A$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M$1:M$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5 M1:M4 M6:M1048576">
       <formula1>'Data Mapping'!$C:$C</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N$1:N$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5 N1:N4 N6:N1048576">
       <formula1>'Data Mapping'!$D:$D</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S$1:S$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S5 S1:S4 S6:S1048576">
       <formula1>'Data Mapping'!$L:$L</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T$1:T$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T5 T1:T4 T6:T1048576">
       <formula1>'Data Mapping'!$J:$J</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U$1:U$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U5 U1:U4 U6:U1048576">
       <formula1>'Data Mapping'!$K:$K</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z$1:Z$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z5 Z1:Z4 Z6:Z1048576">
       <formula1>'Data Mapping'!$S:$S</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA$1:AA$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA5 AA1:AA4 AA6:AA1048576">
       <formula1>'Data Mapping'!$T:$T</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD$1:AD$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD5 AD1:AD4 AD6:AD1048576">
       <formula1>'Data Mapping'!$U:$U</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL$1:AL$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF5:AG5 AF1:AG4 AF6:AG1048576">
+      <formula1>Privacy_Policy</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL5 AL1:AL4 AL6:AL1048576">
       <formula1>'Data Mapping'!$I:$I</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF$1:AG$1048576">
-      <formula1>Privacy_Policy</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3707,7 +3864,7 @@
         <v>8</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>203</v>
@@ -3727,7 +3884,7 @@
     </row>
     <row r="2" spans="1:28">
       <c r="A2" s="2" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -3778,7 +3935,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -3807,7 +3964,7 @@
     </row>
     <row r="3" spans="1:28">
       <c r="A3" s="2" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -3858,7 +4015,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -4009,16 +4166,16 @@
         <v>8</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>10</v>
@@ -4041,7 +4198,7 @@
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="2" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -4092,7 +4249,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -4119,7 +4276,7 @@
         <v>97</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>219</v>
@@ -4130,7 +4287,7 @@
     </row>
     <row r="3" spans="1:32">
       <c r="A3" s="2" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -4181,7 +4338,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -4204,7 +4361,7 @@
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="2" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>209</v>
@@ -4255,7 +4412,7 @@
         <v>216</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>53</v>
@@ -4328,7 +4485,7 @@
   <sheetPr/>
   <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -4413,13 +4570,13 @@
         <v>17</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>10</v>
@@ -4442,7 +4599,7 @@
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="2" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -4493,7 +4650,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -4511,7 +4668,7 @@
         <v>36</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>32</v>
@@ -4523,7 +4680,7 @@
         <v>97</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>219</v>
@@ -4534,7 +4691,7 @@
     </row>
     <row r="3" spans="1:32">
       <c r="A3" s="2" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -4585,7 +4742,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -4611,7 +4768,7 @@
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="2" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>209</v>
@@ -4662,7 +4819,7 @@
         <v>216</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>53</v>
@@ -4688,41 +4845,41 @@
     </row>
   </sheetData>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4 D1:D3 D5:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D$1:D$1048576">
       <formula1>'Data Mapping'!$H:$H</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4 J1:J3 J5:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J$1:J$1048576">
       <formula1>'Data Mapping'!$F:$F</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4 K1:K3 K5:K1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K$1:K$1048576">
       <formula1>'Data Mapping'!$E:$E</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4 L1:L3 L5:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L$1:L$1048576">
       <formula1>'Data Mapping'!$A$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M4 M1:M3 M5:M1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M$1:M$1048576">
       <formula1>'Data Mapping'!$C:$C</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N4 N1:N3 N5:N1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N$1:N$1048576">
       <formula1>'Data Mapping'!$D:$D</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S4 S1:S3 S5:S1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S$1:S$1048576">
       <formula1>'Data Mapping'!$L:$L</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T4 T1:T3 T5:T1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T$1:T$1048576">
       <formula1>'Data Mapping'!$J:$J</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U4 U1:U3 U5:U1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U$1:U$1048576">
       <formula1>'Data Mapping'!$K:$K</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V4 V1:V3 V5:V1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V$1:V$1048576">
       <formula1>'Data Mapping'!$W:$W</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z4:AA4 Z1:AA3 Z5:AA1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF$1:AF$1048576">
+      <formula1>'Data Mapping'!$I:$I</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z$1:AA$1048576">
       <formula1>Privacy_Policy</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF4 AF1:AF3 AF5:AF1048576">
-      <formula1>'Data Mapping'!$I:$I</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4819,7 +4976,7 @@
         <v>18</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>19</v>
@@ -4848,7 +5005,7 @@
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="2" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -4899,7 +5056,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -4917,7 +5074,7 @@
         <v>36</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>42</v>
@@ -4932,7 +5089,7 @@
         <v>97</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>219</v>
@@ -4943,7 +5100,7 @@
     </row>
     <row r="3" spans="1:32">
       <c r="A3" s="2" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -4994,7 +5151,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -5026,7 +5183,7 @@
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="2" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>209</v>
@@ -5077,7 +5234,7 @@
         <v>216</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>53</v>
@@ -5246,7 +5403,7 @@
         <v>8</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>10</v>
@@ -5269,7 +5426,7 @@
     </row>
     <row r="2" spans="1:29">
       <c r="A2" s="2" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -5320,7 +5477,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -5344,7 +5501,7 @@
         <v>97</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="AB2" s="2" t="s">
         <v>219</v>
@@ -5355,7 +5512,7 @@
     </row>
     <row r="3" spans="1:29">
       <c r="A3" s="2" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -5406,7 +5563,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -5429,7 +5586,7 @@
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="2" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>209</v>
@@ -5478,7 +5635,7 @@
         <v>216</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>53</v>
@@ -5640,22 +5797,22 @@
         <v>22</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>10</v>
@@ -5678,7 +5835,7 @@
     </row>
     <row r="2" spans="1:35">
       <c r="A2" s="2" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -5729,7 +5886,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -5744,10 +5901,10 @@
         <v>39</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>32</v>
@@ -5759,7 +5916,7 @@
         <v>97</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="AH2" s="2" t="s">
         <v>219</v>
@@ -5770,10 +5927,10 @@
     </row>
     <row r="3" spans="1:35">
       <c r="A3" s="2" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>210</v>
@@ -5821,7 +5978,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -5836,10 +5993,10 @@
         <v>39</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="AC3" s="2" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
add monitor file code
</commit_message>
<xml_diff>
--- a/SDDI-Metadata.xlsx
+++ b/SDDI-Metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="24750" windowHeight="12200" activeTab="2"/>
+    <workbookView windowWidth="24750" windowHeight="12200" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data Mapping" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="282">
   <si>
     <t>Hauptkategorien</t>
   </si>
@@ -741,6 +741,9 @@
     <t xml:space="preserve">Example Dataset84 </t>
   </si>
   <si>
+    <t>Example Dataset84 84</t>
+  </si>
+  <si>
     <t>This is today dataset</t>
   </si>
   <si>
@@ -840,6 +843,9 @@
     <t>Example Online Application 727</t>
   </si>
   <si>
+    <t>Example Online Application 84</t>
+  </si>
+  <si>
     <t>API Endpoint</t>
   </si>
   <si>
@@ -898,6 +904,9 @@
   </si>
   <si>
     <t>Linux</t>
+  </si>
+  <si>
+    <t>Example Software new test 84</t>
   </si>
 </sst>
 </file>
@@ -1941,7 +1950,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AF33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2644,16 +2653,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:AE6"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="$A6:$XFD6"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="51.75" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.25" style="2" customWidth="1"/>
@@ -3102,8 +3111,8 @@
       <c r="A6" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>226</v>
+      <c r="B6" s="2">
+        <v>84848</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>210</v>
@@ -3175,52 +3184,129 @@
         <v>29</v>
       </c>
     </row>
+    <row r="7" ht="60" customHeight="1" spans="1:31">
+      <c r="A7" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="15">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1 L3:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1 L7 L3:L6 L8:L1048576">
       <formula1>Hauptkategorien</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2">
       <formula1>'Data Mapping'!$A$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D$1:D$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 D1:D6 D8:D1048576">
       <formula1>Lizenzen</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J$1:J$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7 J1:J6 J8:J1048576">
       <formula1>Role</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K$1:K$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7 K1:K6 K8:K1048576">
       <formula1>Organisationen</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M$1:M$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M7 M1:M6 M8:M1048576">
       <formula1>Themen</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N$1:N$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N7 N1:N6 N8:N1048576">
       <formula1>Language</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S$1:S$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S7 S1:S6 S8:S1048576">
       <formula1>Sichtbarkeit</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T$1:T$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T7 T1:T6 T8:T1048576">
       <formula1>Life_Cycle_Phase</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U$1:U$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U7 U1:U6 U8:U1048576">
       <formula1>HOAI_Service_Phase</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V$1:V$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7 V1:V6 V8:V1048576">
       <formula1>Data_Status</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W$1:W$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7 W1:W6 W8:W1048576">
       <formula1>'Data Mapping'!$P:$P</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X$1:X$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7 X1:X6 X8:X1048576">
       <formula1>'Data Mapping'!$Q:$Q</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE$1:AE$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y7:Z7 Y1:Z6 Y8:Z1048576">
+      <formula1>Privacy_Policy</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE7 AE1:AE6 AE8:AE1048576">
       <formula1>Zugriffsrechte</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y$1:Z$1048576">
-      <formula1>Privacy_Policy</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -3236,10 +3322,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AL5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A5" sqref="$A5:$XFD5"/>
@@ -3349,16 +3435,16 @@
         <v>8</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>14</v>
@@ -3367,16 +3453,16 @@
         <v>15</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>10</v>
@@ -3399,7 +3485,7 @@
     </row>
     <row r="2" ht="44" customHeight="1" spans="1:38">
       <c r="A2" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -3450,7 +3536,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -3468,7 +3554,7 @@
         <v>37</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AD2" s="2" t="s">
         <v>38</v>
@@ -3494,7 +3580,7 @@
     </row>
     <row r="3" ht="46.5" customHeight="1" spans="1:38">
       <c r="A3" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -3545,7 +3631,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -3574,7 +3660,7 @@
     </row>
     <row r="4" spans="1:38">
       <c r="A4" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>209</v>
@@ -3598,7 +3684,7 @@
         <v>212</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>27</v>
@@ -3616,7 +3702,7 @@
         <v>25</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>29</v>
@@ -3645,7 +3731,7 @@
     </row>
     <row r="5" spans="1:38">
       <c r="A5" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>209</v>
@@ -3669,7 +3755,7 @@
         <v>212</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>27</v>
@@ -3687,7 +3773,7 @@
         <v>25</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>29</v>
@@ -3716,47 +3802,47 @@
     </row>
   </sheetData>
   <dataValidations count="14">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D1:D4 D6:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D$1:D$1048576">
       <formula1>'Data Mapping'!$H:$H</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5 J1:J4 J6:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J$1:J$1048576">
       <formula1>'Data Mapping'!$F:$F</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5 K1:K4 K6:K1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K$1:K$1048576">
       <formula1>'Data Mapping'!$E:$E</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5 L1:L4 L6:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L$1:L$1048576">
       <formula1>'Data Mapping'!$A$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5 M1:M4 M6:M1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M$1:M$1048576">
       <formula1>'Data Mapping'!$C:$C</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5 N1:N4 N6:N1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N$1:N$1048576">
       <formula1>'Data Mapping'!$D:$D</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S5 S1:S4 S6:S1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S$1:S$1048576">
       <formula1>'Data Mapping'!$L:$L</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T5 T1:T4 T6:T1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T$1:T$1048576">
       <formula1>'Data Mapping'!$J:$J</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U5 U1:U4 U6:U1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U$1:U$1048576">
       <formula1>'Data Mapping'!$K:$K</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z5 Z1:Z4 Z6:Z1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z$1:Z$1048576">
       <formula1>'Data Mapping'!$S:$S</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA5 AA1:AA4 AA6:AA1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA$1:AA$1048576">
       <formula1>'Data Mapping'!$T:$T</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD5 AD1:AD4 AD6:AD1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD$1:AD$1048576">
       <formula1>'Data Mapping'!$U:$U</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF5:AG5 AF1:AG4 AF6:AG1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL$1:AL$1048576">
+      <formula1>'Data Mapping'!$I:$I</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF$1:AG$1048576">
       <formula1>Privacy_Policy</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL5 AL1:AL4 AL6:AL1048576">
-      <formula1>'Data Mapping'!$I:$I</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3766,13 +3852,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:AB3"/>
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="R1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L$1:L$1048576"/>
+      <selection pane="bottomLeft" activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
@@ -3787,19 +3873,19 @@
     <col min="12" max="12" width="24.1666666666667" style="2" customWidth="1"/>
     <col min="13" max="13" width="14.5" style="2" customWidth="1"/>
     <col min="14" max="17" width="9" style="2"/>
-    <col min="18" max="18" width="53.25" style="2" customWidth="1"/>
+    <col min="18" max="18" width="62.1666666666667" style="2" customWidth="1"/>
     <col min="19" max="19" width="17.3333333333333" style="2" customWidth="1"/>
     <col min="20" max="20" width="9" style="2"/>
     <col min="21" max="22" width="18.4166666666667" style="2" customWidth="1"/>
-    <col min="23" max="23" width="14.4166666666667" style="2" customWidth="1"/>
-    <col min="24" max="25" width="9" style="2"/>
-    <col min="26" max="26" width="18.75" style="2" customWidth="1"/>
-    <col min="27" max="27" width="9" style="2"/>
-    <col min="28" max="28" width="13" style="2" customWidth="1"/>
-    <col min="29" max="16384" width="9" style="2"/>
+    <col min="23" max="24" width="14.4166666666667" style="2" customWidth="1"/>
+    <col min="25" max="26" width="9" style="2"/>
+    <col min="27" max="27" width="18.75" style="2" customWidth="1"/>
+    <col min="28" max="28" width="9" style="2"/>
+    <col min="29" max="29" width="13" style="2" customWidth="1"/>
+    <col min="30" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:28">
+    <row r="1" s="1" customFormat="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>187</v>
       </c>
@@ -3864,27 +3950,30 @@
         <v>8</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="X1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:29">
       <c r="A2" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -3935,7 +4024,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -3946,25 +4035,28 @@
       <c r="U2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="W2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:29">
       <c r="A3" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -4015,7 +4107,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -4026,12 +4118,15 @@
       <c r="U3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="W3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC3" s="2" t="s">
         <v>184</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="10">
+  <dataValidations count="11">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D$1:D$1048576">
       <formula1>'Data Mapping'!$H:$H</formula1>
     </dataValidation>
@@ -4059,7 +4154,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U$1:U$1048576">
       <formula1>'Data Mapping'!$K:$K</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB$1:AB$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W1:W4">
+      <formula1>Privacy_Policy</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC$1:AC$1048576">
       <formula1>'Data Mapping'!$I:$I</formula1>
     </dataValidation>
   </dataValidations>
@@ -4070,13 +4168,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="R1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="Z6" sqref="Z6"/>
+      <selection pane="bottomLeft" activeCell="Z1" sqref="Z1:Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
@@ -4166,16 +4264,16 @@
         <v>8</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>10</v>
@@ -4198,7 +4296,7 @@
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -4249,7 +4347,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -4276,7 +4374,7 @@
         <v>97</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>219</v>
@@ -4287,7 +4385,7 @@
     </row>
     <row r="3" spans="1:32">
       <c r="A3" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -4338,7 +4436,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -4361,7 +4459,7 @@
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>209</v>
@@ -4412,7 +4510,7 @@
         <v>216</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>53</v>
@@ -4482,14 +4580,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:AF4"/>
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4"/>
   <cols>
     <col min="1" max="1" width="16.1666666666667" style="2" customWidth="1"/>
     <col min="2" max="3" width="9" style="2"/>
@@ -4570,13 +4668,13 @@
         <v>17</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>10</v>
@@ -4599,7 +4697,7 @@
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -4650,7 +4748,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -4668,7 +4766,7 @@
         <v>36</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>32</v>
@@ -4680,7 +4778,7 @@
         <v>97</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>219</v>
@@ -4691,7 +4789,7 @@
     </row>
     <row r="3" spans="1:32">
       <c r="A3" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -4742,7 +4840,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -4768,7 +4866,7 @@
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>209</v>
@@ -4819,7 +4917,7 @@
         <v>216</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>53</v>
@@ -4840,6 +4938,83 @@
         <v>32</v>
       </c>
       <c r="AF4" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32">
+      <c r="A5" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF5" s="2" t="s">
         <v>184</v>
       </c>
     </row>
@@ -4889,16 +5064,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="21" width="9" style="2"/>
+    <col min="1" max="1" width="36.25" style="2" customWidth="1"/>
+    <col min="2" max="21" width="9" style="2"/>
     <col min="22" max="22" width="18.5" style="2" customWidth="1"/>
     <col min="23" max="23" width="15.75" style="2" customWidth="1"/>
     <col min="24" max="24" width="14.9166666666667" style="2" customWidth="1"/>
@@ -4976,7 +5152,7 @@
         <v>18</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>19</v>
@@ -5005,7 +5181,7 @@
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -5056,7 +5232,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -5074,7 +5250,7 @@
         <v>36</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>42</v>
@@ -5089,7 +5265,7 @@
         <v>97</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>219</v>
@@ -5100,7 +5276,7 @@
     </row>
     <row r="3" spans="1:32">
       <c r="A3" s="2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -5151,7 +5327,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -5183,7 +5359,7 @@
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>209</v>
@@ -5234,7 +5410,7 @@
         <v>216</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>53</v>
@@ -5316,7 +5492,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5403,7 +5579,7 @@
         <v>8</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>10</v>
@@ -5426,7 +5602,7 @@
     </row>
     <row r="2" spans="1:29">
       <c r="A2" s="2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -5477,7 +5653,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -5501,7 +5677,7 @@
         <v>97</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AB2" s="2" t="s">
         <v>219</v>
@@ -5512,7 +5688,7 @@
     </row>
     <row r="3" spans="1:29">
       <c r="A3" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>209</v>
@@ -5563,7 +5739,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -5586,7 +5762,7 @@
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>209</v>
@@ -5635,7 +5811,7 @@
         <v>216</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>53</v>
@@ -5702,14 +5878,14 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:AI3"/>
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:AI4"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AF5" sqref="AF5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="$A4:$XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
   <cols>
     <col min="1" max="1" width="30.3333333333333" style="2" customWidth="1"/>
     <col min="2" max="2" width="31.4166666666667" style="2" customWidth="1"/>
@@ -5797,22 +5973,22 @@
         <v>22</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>10</v>
@@ -5835,7 +6011,7 @@
     </row>
     <row r="2" spans="1:35">
       <c r="A2" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>209</v>
@@ -5886,7 +6062,7 @@
         <v>216</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>29</v>
@@ -5901,10 +6077,10 @@
         <v>39</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>32</v>
@@ -5916,7 +6092,7 @@
         <v>97</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AH2" s="2" t="s">
         <v>219</v>
@@ -5927,10 +6103,10 @@
     </row>
     <row r="3" spans="1:35">
       <c r="A3" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>210</v>
@@ -5978,7 +6154,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
@@ -5993,10 +6169,10 @@
         <v>39</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="AC3" s="2" t="s">
         <v>32</v>
@@ -6011,6 +6187,95 @@
         <v>218</v>
       </c>
       <c r="AI3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35">
+      <c r="A4" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="AI4" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>